<commit_message>
Added linearity, calver, and QC precision data
</commit_message>
<xml_diff>
--- a/data/Method_Validation.data.xlsx
+++ b/data/Method_Validation.data.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="3"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="25860" windowHeight="16420" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MS HCG" sheetId="1" r:id="rId1"/>
     <sheet name="MS AFP" sheetId="2" r:id="rId2"/>
     <sheet name="MS uE3" sheetId="3" r:id="rId3"/>
     <sheet name="Precision" sheetId="4" r:id="rId4"/>
+    <sheet name="Linearity" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Precision!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Precision!$A$1:$G$60</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="478">
   <si>
     <t>Spec ID</t>
   </si>
@@ -1421,35 +1422,62 @@
     <t>P4</t>
   </si>
   <si>
-    <t>The Roche 5th generation troponin assay was recently approved by the FDA. This is simulated data that matches the performance of this assay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The "Blank" is a specimen with no troponin. The others are reference specimens have varying levels of troponin. </t>
-  </si>
-  <si>
-    <t>Each specimen was assayed repeatedly over the course of several days, to estimate the assay intermediate precision, or assay inter-day precision.</t>
-  </si>
-  <si>
-    <t>FDA documents:</t>
-  </si>
-  <si>
-    <t>http://www.accessdata.fda.gov/scripts/cdrh/cfdocs/cfPMN/pmn.cfm?ID=K162895</t>
-  </si>
-  <si>
-    <t>1) Calculate the imprecision at each test level</t>
-  </si>
-  <si>
-    <t>2) What is the limit of the blank? (Although in class we said 2SDs, this is generally defined as the 95th percentile of test results for a blank sample)</t>
-  </si>
-  <si>
-    <t>3) What is the apparent lower limit of quantification (CV ~ 20%)?</t>
+    <t>Result_2</t>
+  </si>
+  <si>
+    <t>Result_1</t>
+  </si>
+  <si>
+    <t>Result_3</t>
+  </si>
+  <si>
+    <t>Assigned_Value</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>AFP</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>90% S6</t>
+  </si>
+  <si>
+    <t>hCG</t>
+  </si>
+  <si>
+    <t>Analyte</t>
+  </si>
+  <si>
+    <t>uE3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1480,6 +1508,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1503,17 +1539,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -6883,1271 +6921,1248 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="3"/>
-    <col min="8" max="8" width="14.83203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="11" style="3"/>
+    <col min="1" max="1" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="4"/>
+    <col min="9" max="9" width="14.83203125" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D2" s="4">
+        <v>7.97</v>
+      </c>
+      <c r="E2" s="4">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7.65</v>
+      </c>
+      <c r="E3" s="4">
+        <v>26.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D4" s="4">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="E4" s="4">
+        <v>25.19</v>
+      </c>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E5" s="4">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8.52</v>
+      </c>
+      <c r="E6" s="4">
+        <v>26.04</v>
+      </c>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D7" s="4">
+        <v>8.23</v>
+      </c>
+      <c r="E7" s="4">
+        <v>25.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D8" s="4">
+        <v>8.61</v>
+      </c>
+      <c r="E8" s="4">
+        <v>25.82</v>
+      </c>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" s="4">
+        <v>7.93</v>
+      </c>
+      <c r="E9" s="4">
+        <v>25.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D10" s="4">
+        <v>8.31</v>
+      </c>
+      <c r="E10" s="4">
+        <v>27.25</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="E11" s="4">
+        <v>26.14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D12" s="4">
+        <v>7.18</v>
+      </c>
+      <c r="E12" s="4">
+        <v>24.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7.48</v>
+      </c>
+      <c r="E13" s="4">
+        <v>23.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D14" s="4">
+        <v>7.7</v>
+      </c>
+      <c r="E14" s="4">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D15" s="4">
+        <v>8.86</v>
+      </c>
+      <c r="E15" s="4">
+        <v>25.29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D16" s="4">
+        <v>7.24</v>
+      </c>
+      <c r="E16" s="4">
+        <v>23.84</v>
+      </c>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D17" s="4">
+        <v>7.79</v>
+      </c>
+      <c r="E17" s="4">
+        <v>24.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D18" s="4">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="E18" s="4">
+        <v>24.64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D19" s="4">
+        <v>7.74</v>
+      </c>
+      <c r="E19" s="4">
+        <v>24.32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D20" s="4">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4">
+        <v>26.68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D21" s="4">
+        <v>7.48</v>
+      </c>
+      <c r="E21" s="4">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D22" s="4">
+        <v>7.92</v>
+      </c>
+      <c r="E22" s="4">
+        <v>25.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D23" s="4">
+        <v>7.58</v>
+      </c>
+      <c r="E23" s="4">
+        <v>25.96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D24" s="4">
+        <v>7.61</v>
+      </c>
+      <c r="E24" s="4">
+        <v>26.53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D25" s="4">
+        <v>8.34</v>
+      </c>
+      <c r="E25" s="4">
+        <v>25.57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D26" s="4">
+        <v>7.76</v>
+      </c>
+      <c r="E26" s="4">
+        <v>25.72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D27" s="4">
+        <v>7.61</v>
+      </c>
+      <c r="E27" s="4">
+        <v>27.89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D28" s="4">
+        <v>8.26</v>
+      </c>
+      <c r="E28" s="4">
+        <v>27.68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D29" s="4">
+        <v>8.49</v>
+      </c>
+      <c r="E29" s="4">
+        <v>26.83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D30" s="4">
+        <v>8.09</v>
+      </c>
+      <c r="E30" s="4">
+        <v>27.78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D31" s="4">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="E31" s="4">
+        <v>26.93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>32</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="F32" s="4">
+        <v>5.6820000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="F33" s="4">
+        <v>5.6959999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="F34" s="4">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="F35" s="4">
+        <v>6.0730000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>36</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.435</v>
+      </c>
+      <c r="F36" s="4">
+        <v>5.5339999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="F37" s="4">
+        <v>5.5149999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="F38" s="4">
+        <v>5.8449999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F39" s="4">
+        <v>5.6070000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>40</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F40" s="4">
+        <v>5.5449999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>41</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="F41" s="4">
+        <v>5.681</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>42</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="F42" s="4">
+        <v>5.4409999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>43</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="F43" s="4">
+        <v>5.4690000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.436</v>
+      </c>
+      <c r="F44" s="4">
+        <v>5.3209999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>45</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="F45" s="4">
+        <v>5.867</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>46</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.434</v>
+      </c>
+      <c r="F46" s="4">
+        <v>5.5750000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.435</v>
+      </c>
+      <c r="F47" s="4">
+        <v>5.2460000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>48</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="F48" s="4">
+        <v>5.3109999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>49</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0.438</v>
+      </c>
+      <c r="F49" s="4">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>50</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="F50" s="4">
+        <v>5.3330000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>51</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.437</v>
+      </c>
+      <c r="F51" s="4">
+        <v>5.6349999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>52</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="F52" s="4">
+        <v>5.5960000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>53</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="F53" s="4">
+        <v>5.6340000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>54</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="F54" s="4">
+        <v>5.5960000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>55</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="F55" s="4">
+        <v>5.6340000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>56</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="F56" s="4">
+        <v>5.9039999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>57</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="F57" s="4">
+        <v>5.5570000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="F58" s="4">
+        <v>5.4630000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>59</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="F59" s="4">
+        <v>5.3869999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>60</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0.435</v>
+      </c>
+      <c r="F60" s="4">
+        <v>5.3860000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4">
+        <v>61</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="F61" s="4">
+        <v>5.5810000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G60"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="6" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C2" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="D2" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="E2" s="3">
-        <v>22.5</v>
+      <c r="E1" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.03</v>
       </c>
       <c r="F2" s="3">
-        <v>105</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B3" t="s">
+        <v>467</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.71</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.64</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.09</v>
+      </c>
+      <c r="F3" s="3">
         <v>2.5</v>
       </c>
-      <c r="C3" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>8.1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>22.5</v>
-      </c>
-      <c r="F3" s="3">
-        <v>96.3</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3">
-        <v>19</v>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5.91</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.08</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.98</v>
       </c>
       <c r="F4" s="3">
-        <v>98.6</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="E5" s="3">
-        <v>18.399999999999999</v>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B5" t="s">
+        <v>467</v>
+      </c>
+      <c r="C5" s="2">
+        <v>30.29</v>
+      </c>
+      <c r="D5" s="2">
+        <v>29.54</v>
+      </c>
+      <c r="E5" s="2">
+        <v>31.71</v>
       </c>
       <c r="F5" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C6" s="2">
+        <v>122.97</v>
+      </c>
+      <c r="D6" s="2">
+        <v>117.89</v>
+      </c>
+      <c r="E6" s="2">
+        <v>116.8</v>
+      </c>
+      <c r="F6" s="3">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="C6" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="F6" s="3">
-        <v>107.2</v>
-      </c>
-      <c r="H6" s="5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B7" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5.8</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="2">
+        <v>569.23</v>
+      </c>
+      <c r="D7" s="2">
+        <v>575.66</v>
+      </c>
+      <c r="E7" s="2">
+        <v>573.08000000000004</v>
+      </c>
+      <c r="F7" s="3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B8" t="s">
+        <v>467</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2913.8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2970.2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2756.2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" t="s">
+        <v>475</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5.74</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.88</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5.85</v>
+      </c>
+      <c r="F10" s="2">
         <v>5.7</v>
       </c>
-      <c r="E7" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>101.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="C8" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="E8" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="F8" s="3">
-        <v>93.8</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C9" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="F9" s="3">
-        <v>102.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C10" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="D10" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E10" s="3">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="F10" s="3">
-        <v>101.2</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="E11" s="3">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="F11" s="3">
-        <v>95.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="E12" s="3">
-        <v>21.6</v>
-      </c>
-      <c r="F12" s="3">
-        <v>105.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="C13" s="3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D13" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="E13" s="3">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="F13" s="3">
-        <v>106.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C14" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="D14" s="3">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E14" s="3">
-        <v>21</v>
-      </c>
-      <c r="F14" s="3">
-        <v>97.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="C15" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="D15" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="E15" s="3">
-        <v>23.6</v>
-      </c>
-      <c r="F15" s="3">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="C16" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="D16" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="E16" s="3">
-        <v>20.3</v>
-      </c>
-      <c r="F16" s="3">
-        <v>98.1</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C17" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="D17" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="E17" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="F17" s="3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="C18" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="D18" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="E18" s="3">
-        <v>18.3</v>
-      </c>
-      <c r="F18" s="3">
-        <v>100.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="C19" s="3">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3">
-        <v>5.8</v>
-      </c>
-      <c r="E19" s="3">
-        <v>19.5</v>
-      </c>
-      <c r="F19" s="3">
-        <v>92.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="E20" s="3">
-        <v>18.7</v>
-      </c>
-      <c r="F20" s="3">
-        <v>97.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C21" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="D21" s="3">
-        <v>5.9</v>
-      </c>
-      <c r="E21" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="F21" s="3">
-        <v>97.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="C22" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="D22" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="E22" s="3">
-        <v>21.4</v>
-      </c>
-      <c r="F22" s="3">
-        <v>102.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C23" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="D23" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="E23" s="3">
-        <v>21.3</v>
-      </c>
-      <c r="F23" s="3">
-        <v>96.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1.7</v>
-      </c>
-      <c r="C24" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="D24" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="E24" s="3">
-        <v>22.7</v>
-      </c>
-      <c r="F24" s="3">
-        <v>102.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="C25" s="3">
-        <v>4</v>
-      </c>
-      <c r="D25" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="E25" s="3">
-        <v>18.7</v>
-      </c>
-      <c r="F25" s="3">
-        <v>95.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="C26" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="D26" s="3">
-        <v>4</v>
-      </c>
-      <c r="E26" s="3">
-        <v>21.4</v>
-      </c>
-      <c r="F26" s="3">
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C27" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="D27" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="E27" s="3">
-        <v>18.8</v>
-      </c>
-      <c r="F27" s="3">
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="C28" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="D28" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="E28" s="3">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="F28" s="3">
-        <v>94.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="C29" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="D29" s="3">
-        <v>7</v>
-      </c>
-      <c r="E29" s="3">
-        <v>21.3</v>
-      </c>
-      <c r="F29" s="3">
-        <v>100.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C30" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="D30" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="E30" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="F30" s="3">
-        <v>105.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>30</v>
-      </c>
-      <c r="B31" s="3">
-        <v>2</v>
-      </c>
-      <c r="C31" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="E31" s="3">
-        <v>18.8</v>
-      </c>
-      <c r="F31" s="3">
-        <v>103.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>31</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="C32" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="D32" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="E32" s="3">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="F32" s="3">
-        <v>93.2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C33" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D33" s="3">
-        <v>5.3</v>
-      </c>
-      <c r="E33" s="3">
-        <v>22</v>
-      </c>
-      <c r="F33" s="3">
-        <v>101.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
-        <v>33</v>
-      </c>
-      <c r="B34" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="C34" s="3">
-        <v>5.3</v>
-      </c>
-      <c r="D34" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="E34" s="3">
-        <v>23.3</v>
-      </c>
-      <c r="F34" s="3">
-        <v>93.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>470</v>
+      </c>
+      <c r="B11" t="s">
+        <v>475</v>
+      </c>
+      <c r="C11" s="2">
+        <v>32.07</v>
+      </c>
+      <c r="D11" s="2">
+        <v>32.64</v>
+      </c>
+      <c r="E11" s="2">
+        <v>34.15</v>
+      </c>
+      <c r="F11" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="C35" s="3">
-        <v>5.3</v>
-      </c>
-      <c r="D35" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="E35" s="3">
-        <v>21.1</v>
-      </c>
-      <c r="F35" s="3">
-        <v>96.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C36" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="D36" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="E36" s="3">
-        <v>19.2</v>
-      </c>
-      <c r="F36" s="3">
-        <v>98.4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C37" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="D37" s="3">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="F37" s="3">
-        <v>105.6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
-        <v>37</v>
-      </c>
-      <c r="B38" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C38" s="3">
-        <v>5.6</v>
-      </c>
-      <c r="D38" s="3">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3">
-        <v>19.2</v>
-      </c>
-      <c r="F38" s="3">
-        <v>102.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <v>38</v>
-      </c>
-      <c r="B39" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="C39" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D39" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="E39" s="3">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="F39" s="3">
-        <v>101.2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <v>39</v>
-      </c>
-      <c r="B40" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C40" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="D40" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="E40" s="3">
-        <v>20.8</v>
-      </c>
-      <c r="F40" s="3">
-        <v>100.7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
-        <v>40</v>
-      </c>
-      <c r="B41" s="3">
-        <v>2</v>
-      </c>
-      <c r="C41" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="D41" s="3">
-        <v>8.1</v>
-      </c>
-      <c r="E41" s="3">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="F41" s="3">
-        <v>109.3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="C42" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D42" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="E42" s="3">
-        <v>20.9</v>
-      </c>
-      <c r="F42" s="3">
-        <v>99.1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <v>42</v>
-      </c>
-      <c r="B43" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C43" s="3">
-        <v>5.3</v>
-      </c>
-      <c r="D43" s="3">
-        <v>5</v>
-      </c>
-      <c r="E43" s="3">
-        <v>19.3</v>
-      </c>
-      <c r="F43" s="3">
-        <v>99.1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="C44" s="3">
-        <v>2.7</v>
-      </c>
-      <c r="D44" s="3">
-        <v>7</v>
-      </c>
-      <c r="E44" s="3">
-        <v>19</v>
-      </c>
-      <c r="F44" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="C45" s="3">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D45" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="E45" s="3">
-        <v>20.7</v>
-      </c>
-      <c r="F45" s="3">
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
-        <v>45</v>
-      </c>
-      <c r="B46" s="3">
-        <v>-0.2</v>
-      </c>
-      <c r="C46" s="3">
-        <v>6</v>
-      </c>
-      <c r="D46" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="E46" s="3">
-        <v>22</v>
-      </c>
-      <c r="F46" s="3">
-        <v>97.9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>46</v>
-      </c>
-      <c r="B47" s="3">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="D47" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E47" s="3">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="F47" s="3">
-        <v>94.7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
-        <v>47</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1.7</v>
-      </c>
-      <c r="C48" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="D48" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="E48" s="3">
-        <v>20.2</v>
-      </c>
-      <c r="F48" s="3">
-        <v>99.3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
-        <v>48</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="C49" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="D49" s="3">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E49" s="3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="F49" s="3">
-        <v>98.6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
-        <v>49</v>
-      </c>
-      <c r="B50" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="C50" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="D50" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="E50" s="3">
-        <v>19</v>
-      </c>
-      <c r="F50" s="3">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="3">
-        <v>50</v>
-      </c>
-      <c r="B51" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="C51" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="D51" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="E51" s="3">
-        <v>19</v>
-      </c>
-      <c r="F51" s="3">
-        <v>103.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C52" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D52" s="3">
-        <v>5.6</v>
-      </c>
-      <c r="E52" s="3">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="F52" s="3">
-        <v>97.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
-        <v>52</v>
-      </c>
-      <c r="B53" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="C53" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="D53" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="E53" s="3">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="F53" s="3">
-        <v>101.6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="3">
-        <v>53</v>
-      </c>
-      <c r="B54" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="C54" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="D54" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="E54" s="3">
-        <v>21.8</v>
-      </c>
-      <c r="F54" s="3">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
-        <v>54</v>
-      </c>
-      <c r="B55" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="C55" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D55" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="E55" s="3">
-        <v>20.8</v>
-      </c>
-      <c r="F55" s="3">
-        <v>100.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
-        <v>55</v>
-      </c>
-      <c r="B56" s="3">
-        <v>2</v>
-      </c>
-      <c r="C56" s="3">
-        <v>5.6</v>
-      </c>
-      <c r="D56" s="3">
-        <v>5.8</v>
-      </c>
-      <c r="E56" s="3">
-        <v>22.6</v>
-      </c>
-      <c r="F56" s="3">
-        <v>103.2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
-        <v>56</v>
-      </c>
-      <c r="B57" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="C57" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="D57" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="E57" s="3">
-        <v>20.7</v>
-      </c>
-      <c r="F57" s="3">
-        <v>98.1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
-        <v>57</v>
-      </c>
-      <c r="B58" s="3">
-        <v>-0.4</v>
-      </c>
-      <c r="C58" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D58" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="E58" s="3">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="F58" s="3">
-        <v>100.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
-        <v>58</v>
-      </c>
-      <c r="B59" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="C59" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="D59" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="E59" s="3">
-        <v>20.2</v>
-      </c>
-      <c r="F59" s="3">
-        <v>105.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
-        <v>59</v>
-      </c>
-      <c r="B60" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="C60" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="D60" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="E60" s="3">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="F60" s="3">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="C61" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="D61" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="E61" s="3">
-        <v>21.3</v>
-      </c>
-      <c r="F61" s="3">
-        <v>92.3</v>
-      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12" t="s">
+        <v>475</v>
+      </c>
+      <c r="C12" s="2">
+        <v>194.46</v>
+      </c>
+      <c r="D12" s="2">
+        <v>195.69</v>
+      </c>
+      <c r="E12" s="2">
+        <v>197.41</v>
+      </c>
+      <c r="F12" s="2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>472</v>
+      </c>
+      <c r="B13" t="s">
+        <v>475</v>
+      </c>
+      <c r="C13" s="2">
+        <v>559.52</v>
+      </c>
+      <c r="D13" s="2">
+        <v>592.29</v>
+      </c>
+      <c r="E13" s="2">
+        <v>587.5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B14" t="s">
+        <v>475</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1293.3499999999999</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1288.96</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1311.35</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F61"/>
-  <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>